<commit_message>
[UPDATE] setup.cfg with requirements + location of DFA scripts + scripts for diel tomato model and validations + [ADD] photoautotrophic conditions file
</commit_message>
<xml_diff>
--- a/Validation/produced_at_day_tomato.xlsx
+++ b/Validation/produced_at_day_tomato.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E3"/>
+  <dimension ref="B1:E1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -455,44 +455,6 @@
         </is>
       </c>
     </row>
-    <row r="2">
-      <c r="A2" s="1" t="inlineStr">
-        <is>
-          <t>GLN_Cyto_Day_sp_exchange</t>
-        </is>
-      </c>
-      <c r="B2" t="n">
-        <v>0.0001030480760380033</v>
-      </c>
-      <c r="C2" t="n">
-        <v>-1000000</v>
-      </c>
-      <c r="D2" t="n">
-        <v>999999.9999999993</v>
-      </c>
-      <c r="E2" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" s="1" t="inlineStr">
-        <is>
-          <t>CIT_Cyto_Day_sp_exchange</t>
-        </is>
-      </c>
-      <c r="B3" t="n">
-        <v>9.110192436833468e-05</v>
-      </c>
-      <c r="C3" t="n">
-        <v>-999999.9999999999</v>
-      </c>
-      <c r="D3" t="n">
-        <v>999999.9999999999</v>
-      </c>
-      <c r="E3" t="b">
-        <v>0</v>
-      </c>
-    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>